<commit_message>
udpated the test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/XLSXFiles/testpage.xlsx
+++ b/src/test/resources/XLSXFiles/testpage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="180">
   <si>
     <t xml:space="preserve">ELEMENT_NAME</t>
   </si>
@@ -520,6 +520,48 @@
   </si>
   <si>
     <t>Ali</t>
+  </si>
+  <si>
+    <t>Catheryn</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Troy</t>
+  </si>
+  <si>
+    <t>Camilla</t>
+  </si>
+  <si>
+    <t>Trent</t>
+  </si>
+  <si>
+    <t>Perry</t>
+  </si>
+  <si>
+    <t>Norbert</t>
+  </si>
+  <si>
+    <t>Mickey</t>
+  </si>
+  <si>
+    <t>Jerrod</t>
+  </si>
+  <si>
+    <t>Ron</t>
+  </si>
+  <si>
+    <t>Gidget</t>
+  </si>
+  <si>
+    <t>Lynna</t>
+  </si>
+  <si>
+    <t>Ena</t>
+  </si>
+  <si>
+    <t>Jeannetta</t>
   </si>
 </sst>
 </file>
@@ -918,57 +960,57 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="1">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s" s="1">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="1">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s" s="1">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s" s="1">
-        <v>159</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="1">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s" s="1">
-        <v>156</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s" s="1">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s" s="1">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s" s="1">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="B6" t="s" s="1">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="C6" t="s" s="1">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the testNG xml
</commit_message>
<xml_diff>
--- a/src/test/resources/XLSXFiles/testpage.xlsx
+++ b/src/test/resources/XLSXFiles/testpage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t xml:space="preserve">ELEMENT_NAME</t>
   </si>
@@ -90,271 +90,91 @@
     <t xml:space="preserve">Six</t>
   </si>
   <si>
-    <t xml:space="preserve">Zana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bartoletti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gerbil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(520) 318-4711</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Illinois College</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Traralgon – Morwell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">King</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mosquito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(434) 661-5931</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North West</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sydney</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schmidt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caribou</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(309) 501-0792</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North Nienow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toowoomba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sadye</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daugherty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(479) 925-0034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nolan Academy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mackay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anibal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greenfelder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cockroach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(830) 210-1843 x5056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moore University</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bunbury</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Gerardo</t>
-  </si>
-  <si>
-    <t>Sporer</t>
-  </si>
-  <si>
-    <t>hound</t>
-  </si>
-  <si>
-    <t>(765) 828-0379 x8125</t>
-  </si>
-  <si>
-    <t>North Streich</t>
-  </si>
-  <si>
-    <t>Bendigo</t>
-  </si>
-  <si>
-    <t>Madge</t>
-  </si>
-  <si>
-    <t>Leuschke</t>
-  </si>
-  <si>
-    <t>squirrel</t>
-  </si>
-  <si>
-    <t>(434) 610-7551</t>
-  </si>
-  <si>
-    <t>South Goyette</t>
-  </si>
-  <si>
-    <t>Albury</t>
-  </si>
-  <si>
-    <t>Benito</t>
-  </si>
-  <si>
-    <t>Waelchi</t>
-  </si>
-  <si>
-    <t>ant</t>
-  </si>
-  <si>
-    <t>(404) 618-5376 x8315</t>
-  </si>
-  <si>
-    <t>Southern Maine University</t>
-  </si>
-  <si>
-    <t>Tamworth</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Luettgen</t>
-  </si>
-  <si>
-    <t>cricket</t>
-  </si>
-  <si>
-    <t>(626) 410-8351</t>
-  </si>
-  <si>
-    <t>Bernhard Academy</t>
-  </si>
-  <si>
-    <t>Kalgoorlie</t>
-  </si>
-  <si>
-    <t>Edgardo</t>
-  </si>
-  <si>
-    <t>Olson</t>
-  </si>
-  <si>
-    <t>wildebeest</t>
-  </si>
-  <si>
-    <t>(207) 614-7703 x9844</t>
-  </si>
-  <si>
-    <t>South Kertzmann College</t>
-  </si>
-  <si>
-    <t>Townsville</t>
-  </si>
-  <si>
-    <t>Jeana</t>
-  </si>
-  <si>
-    <t>Feest</t>
-  </si>
-  <si>
-    <t>jellyfish</t>
-  </si>
-  <si>
-    <t>(347) 251-8515</t>
-  </si>
-  <si>
-    <t>North Schuppe College</t>
-  </si>
-  <si>
-    <t>Sydney</t>
-  </si>
-  <si>
-    <t>Salvatore</t>
-  </si>
-  <si>
-    <t>porcupine</t>
-  </si>
-  <si>
-    <t>(347) 706-8023 x0637</t>
-  </si>
-  <si>
-    <t>North North Dakota College</t>
-  </si>
-  <si>
-    <t>Hobart</t>
-  </si>
-  <si>
-    <t>Fay</t>
-  </si>
-  <si>
-    <t>Osinski</t>
-  </si>
-  <si>
-    <t>hyena</t>
-  </si>
-  <si>
-    <t>(256) 801-8827 x8572</t>
-  </si>
-  <si>
-    <t>The Harvey College</t>
-  </si>
-  <si>
-    <t>Wagga	Wagga</t>
-  </si>
-  <si>
-    <t>Roosevelt</t>
-  </si>
-  <si>
-    <t>Kling</t>
-  </si>
-  <si>
-    <t>reindeer</t>
-  </si>
-  <si>
-    <t>(623) 904-6161</t>
-  </si>
-  <si>
-    <t>Swift Institute</t>
-  </si>
-  <si>
-    <t>Margo</t>
-  </si>
-  <si>
-    <t>Barrows</t>
-  </si>
-  <si>
-    <t>salmon</t>
-  </si>
-  <si>
-    <t>(614) 754-2682</t>
-  </si>
-  <si>
-    <t>Eastern Gulgowski University</t>
-  </si>
-  <si>
-    <t>Port Macquarie</t>
+    <t xml:space="preserve">Stephany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuhn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wallaby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(620) 620-0455 x7183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Macejkovic College</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Albury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hermiston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(513) 906-0221 x8683</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effertz Institute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bowral – Mittagong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ericka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monahan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turtle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(407) 989-2160 x1767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Anderson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ballarat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jerrell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mallard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(208) 908-4082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Quigley University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunshine Coast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shawn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rhinoceros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(757) 501-2547 x1965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The South Dakota Academy</t>
   </si>
 </sst>
 </file>
@@ -562,10 +382,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="19.17" collapsed="false" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="21.26" collapsed="false" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="41.94" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="1024" customWidth="false" hidden="false" style="1" width="11.57" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,10 +478,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="19.17" collapsed="false" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="21.26" collapsed="false" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="41.94" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="1024" customWidth="false" hidden="false" style="1" width="11.57" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,16 +569,16 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" customWidth="false" hidden="false" style="1" width="11.52" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="26.81" collapsed="false" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="21.67" collapsed="false" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="19.86" collapsed="false" outlineLevel="0"/>
-    <col min="7" max="1024" customWidth="false" hidden="false" style="1" width="11.52" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,45 +601,105 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added testNG thread affinity setup
</commit_message>
<xml_diff>
--- a/src/test/resources/XLSXFiles/testpage.xlsx
+++ b/src/test/resources/XLSXFiles/testpage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="112">
   <si>
     <t xml:space="preserve">ELEMENT_NAME</t>
   </si>
@@ -268,6 +268,96 @@
   </si>
   <si>
     <t>Mount Gambier</t>
+  </si>
+  <si>
+    <t>Danae</t>
+  </si>
+  <si>
+    <t>Hill</t>
+  </si>
+  <si>
+    <t>otter</t>
+  </si>
+  <si>
+    <t>(425) 412-3011 x6305</t>
+  </si>
+  <si>
+    <t>Southern Louisiana Academy</t>
+  </si>
+  <si>
+    <t>Wollongong</t>
+  </si>
+  <si>
+    <t>Venus</t>
+  </si>
+  <si>
+    <t>Bernhard</t>
+  </si>
+  <si>
+    <t>trout</t>
+  </si>
+  <si>
+    <t>(636) 504-0197 x0230</t>
+  </si>
+  <si>
+    <t>Northern Hirthe University</t>
+  </si>
+  <si>
+    <t>Kalgoorlie</t>
+  </si>
+  <si>
+    <t>Ammie</t>
+  </si>
+  <si>
+    <t>D'Amore</t>
+  </si>
+  <si>
+    <t>grasshopper</t>
+  </si>
+  <si>
+    <t>(574) 404-4898</t>
+  </si>
+  <si>
+    <t>Maggio Institute</t>
+  </si>
+  <si>
+    <t>Brisbane</t>
+  </si>
+  <si>
+    <t>Ray</t>
+  </si>
+  <si>
+    <t>Boehm</t>
+  </si>
+  <si>
+    <t>herring</t>
+  </si>
+  <si>
+    <t>(404) 916-7306 x2032</t>
+  </si>
+  <si>
+    <t>Eastern Morissette</t>
+  </si>
+  <si>
+    <t>Central Coast</t>
+  </si>
+  <si>
+    <t>Hershel</t>
+  </si>
+  <si>
+    <t>Dickinson</t>
+  </si>
+  <si>
+    <t>bat</t>
+  </si>
+  <si>
+    <t>(406) 828-4253</t>
+  </si>
+  <si>
+    <t>Stamm College</t>
+  </si>
+  <si>
+    <t>Busselton</t>
   </si>
 </sst>
 </file>
@@ -696,102 +786,102 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="1">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s" s="1">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s" s="1">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s" s="1">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="F2" t="s" s="1">
-        <v>57</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="1">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s" s="1">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s" s="1">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s" s="1">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s" s="1">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s" s="1">
-        <v>63</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="1">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s" s="1">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s" s="1">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s" s="1">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="E4" t="s" s="1">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s" s="1">
-        <v>75</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s" s="1">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s" s="1">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s" s="1">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s" s="1">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s" s="1">
-        <v>69</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s" s="1">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s" s="1">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s" s="1">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s" s="1">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F6" t="s" s="1">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>